<commit_message>
unicode excel error fix
</commit_message>
<xml_diff>
--- a/AstroLinks.xlsx
+++ b/AstroLinks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\albusmw.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77092561-8308-41E9-9842-D30D24E47A8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62385CAC-850E-47EA-B4BF-F68AC80EE959}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10005" yWindow="6585" windowWidth="21465" windowHeight="26235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19980" yWindow="6030" windowWidth="21465" windowHeight="26235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -135,9 +135,6 @@
     <t>(EN) AstroBin</t>
   </si>
   <si>
-    <t>Own products, 10Micron, PWI, …</t>
-  </si>
-  <si>
     <t>Sat images of the sun in multiple wavelengths</t>
   </si>
   <si>
@@ -172,6 +169,9 @@
   </si>
   <si>
     <t>https://sdo.gsfc.nasa.gov</t>
+  </si>
+  <si>
+    <t>Own products, 10Micron, PWI, and others</t>
   </si>
 </sst>
 </file>
@@ -514,7 +514,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -624,7 +624,7 @@
         <v>25</v>
       </c>
       <c r="C9" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>20</v>
@@ -638,10 +638,10 @@
         <v>26</v>
       </c>
       <c r="C10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -649,10 +649,10 @@
         <v>27</v>
       </c>
       <c r="C11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -663,10 +663,10 @@
         <v>28</v>
       </c>
       <c r="C12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -674,10 +674,10 @@
         <v>29</v>
       </c>
       <c r="C13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -688,7 +688,7 @@
         <v>30</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -696,7 +696,7 @@
         <v>34</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -704,10 +704,10 @@
         <v>35</v>
       </c>
       <c r="C16" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>